<commit_message>
Updated SQL & XLSX files for October purchases. Created new SQL tables & files to cater to Platinums and Trophies.
</commit_message>
<xml_diff>
--- a/playstation/output/trophies & platinums.xlsx
+++ b/playstation/output/trophies & platinums.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="2024-10-15" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="2024-10-21" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="trophies" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="platinums" sheetId="3" r:id="rId6"/>
   </sheets>
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="288">
   <si>
     <t>Year</t>
   </si>
@@ -872,6 +872,12 @@
   <si>
     <t>Astro Bot</t>
   </si>
+  <si>
+    <t>Yakuza 0</t>
+  </si>
+  <si>
+    <t>17/10/2024</t>
+  </si>
 </sst>
 </file>
 
@@ -1355,11 +1361,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1117777867"/>
-        <c:axId val="1055773142"/>
+        <c:axId val="549131329"/>
+        <c:axId val="1446847303"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="1117777867"/>
+        <c:axId val="549131329"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1411,10 +1417,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1055773142"/>
+        <c:crossAx val="1446847303"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1055773142"/>
+        <c:axId val="1446847303"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1489,7 +1495,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1117777867"/>
+        <c:crossAx val="549131329"/>
       </c:valAx>
     </c:plotArea>
   </c:chart>
@@ -1526,21 +1532,21 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>platinums!$A$2:$A$170</c:f>
+              <c:f>platinums!$A$2:$A$1000</c:f>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>platinums!$E$2:$E$170</c:f>
+              <c:f>platinums!$E$2:$E$1000</c:f>
               <c:numCache/>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="288379280"/>
-        <c:axId val="2123804871"/>
+        <c:axId val="1277003662"/>
+        <c:axId val="1871282221"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="288379280"/>
+        <c:axId val="1277003662"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1575,7 +1581,7 @@
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="cross"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:spPr/>
         <c:txPr>
@@ -1592,10 +1598,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2123804871"/>
+        <c:crossAx val="1871282221"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2123804871"/>
+        <c:axId val="1871282221"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1670,7 +1676,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="288379280"/>
+        <c:crossAx val="1277003662"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -1717,8 +1723,8 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="14211300" cy="8782050"/>
@@ -2065,19 +2071,19 @@
       </c>
       <c r="L2" s="11">
         <f t="shared" ref="L2:O2" si="1">(G2-G17)+1</f>
-        <v>-22</v>
+        <v>-23</v>
       </c>
       <c r="M2" s="12">
         <f t="shared" si="1"/>
-        <v>-112</v>
+        <v>-113</v>
       </c>
       <c r="N2" s="13">
         <f t="shared" si="1"/>
-        <v>-263</v>
+        <v>-265</v>
       </c>
       <c r="O2" s="14">
         <f t="shared" si="1"/>
-        <v>-857</v>
+        <v>-864</v>
       </c>
       <c r="P2" s="15" t="s">
         <v>6</v>
@@ -2129,19 +2135,19 @@
       </c>
       <c r="L3" s="11">
         <f t="shared" ref="L3:O3" si="2">(G3-G17)+1</f>
-        <v>-22</v>
+        <v>-23</v>
       </c>
       <c r="M3" s="12">
         <f t="shared" si="2"/>
-        <v>-110</v>
+        <v>-111</v>
       </c>
       <c r="N3" s="13">
         <f t="shared" si="2"/>
-        <v>-249</v>
+        <v>-251</v>
       </c>
       <c r="O3" s="14">
         <f t="shared" si="2"/>
-        <v>-771</v>
+        <v>-778</v>
       </c>
       <c r="P3" s="15" t="s">
         <v>8</v>
@@ -2193,19 +2199,19 @@
       </c>
       <c r="L4" s="11">
         <f t="shared" ref="L4:O4" si="3">(G4-G17)+1</f>
-        <v>-22</v>
+        <v>-23</v>
       </c>
       <c r="M4" s="12">
         <f t="shared" si="3"/>
-        <v>-112</v>
+        <v>-113</v>
       </c>
       <c r="N4" s="13">
         <f t="shared" si="3"/>
-        <v>-253</v>
+        <v>-255</v>
       </c>
       <c r="O4" s="14">
         <f t="shared" si="3"/>
-        <v>-803</v>
+        <v>-810</v>
       </c>
       <c r="P4" s="15" t="s">
         <v>5</v>
@@ -2257,19 +2263,19 @@
       </c>
       <c r="L5" s="11">
         <f t="shared" ref="L5:O5" si="4">(G5-G17)+1</f>
-        <v>-21</v>
+        <v>-22</v>
       </c>
       <c r="M5" s="12">
         <f t="shared" si="4"/>
-        <v>-106</v>
+        <v>-107</v>
       </c>
       <c r="N5" s="13">
         <f t="shared" si="4"/>
-        <v>-224</v>
+        <v>-226</v>
       </c>
       <c r="O5" s="14">
         <f t="shared" si="4"/>
-        <v>-744</v>
+        <v>-751</v>
       </c>
       <c r="P5" s="15" t="s">
         <v>10</v>
@@ -2321,19 +2327,19 @@
       </c>
       <c r="L6" s="11">
         <f t="shared" ref="L6:O6" si="5">(G6-G17)+1</f>
-        <v>-22</v>
+        <v>-23</v>
       </c>
       <c r="M6" s="12">
         <f t="shared" si="5"/>
-        <v>-104</v>
+        <v>-105</v>
       </c>
       <c r="N6" s="13">
         <f t="shared" si="5"/>
-        <v>-231</v>
+        <v>-233</v>
       </c>
       <c r="O6" s="14">
         <f t="shared" si="5"/>
-        <v>-636</v>
+        <v>-643</v>
       </c>
       <c r="P6" s="15" t="s">
         <v>9</v>
@@ -2385,19 +2391,19 @@
       </c>
       <c r="L7" s="11">
         <f t="shared" ref="L7:O7" si="6">(G7-G17)+1</f>
-        <v>-22</v>
+        <v>-23</v>
       </c>
       <c r="M7" s="12">
         <f t="shared" si="6"/>
-        <v>-100</v>
+        <v>-101</v>
       </c>
       <c r="N7" s="13">
         <f t="shared" si="6"/>
-        <v>-219</v>
+        <v>-221</v>
       </c>
       <c r="O7" s="14">
         <f t="shared" si="6"/>
-        <v>-654</v>
+        <v>-661</v>
       </c>
       <c r="P7" s="15" t="s">
         <v>11</v>
@@ -2449,19 +2455,19 @@
       </c>
       <c r="L8" s="11">
         <f t="shared" ref="L8:O8" si="7">(G8-G17)+1</f>
-        <v>-20</v>
+        <v>-21</v>
       </c>
       <c r="M8" s="12">
         <f t="shared" si="7"/>
-        <v>-85</v>
+        <v>-86</v>
       </c>
       <c r="N8" s="13">
         <f t="shared" si="7"/>
-        <v>-192</v>
+        <v>-194</v>
       </c>
       <c r="O8" s="14">
         <f t="shared" si="7"/>
-        <v>-546</v>
+        <v>-553</v>
       </c>
       <c r="P8" s="15" t="s">
         <v>12</v>
@@ -2513,19 +2519,19 @@
       </c>
       <c r="L9" s="11">
         <f t="shared" ref="L9:O9" si="8">(G9-G17)+1</f>
-        <v>-21</v>
+        <v>-22</v>
       </c>
       <c r="M9" s="12">
         <f t="shared" si="8"/>
-        <v>-108</v>
+        <v>-109</v>
       </c>
       <c r="N9" s="13">
         <f t="shared" si="8"/>
-        <v>-231</v>
+        <v>-233</v>
       </c>
       <c r="O9" s="14">
         <f t="shared" si="8"/>
-        <v>-789</v>
+        <v>-796</v>
       </c>
       <c r="P9" s="15" t="s">
         <v>7</v>
@@ -2577,19 +2583,19 @@
       </c>
       <c r="L10" s="11">
         <f t="shared" ref="L10:O10" si="9">(G10-G17)+1</f>
-        <v>-20</v>
+        <v>-21</v>
       </c>
       <c r="M10" s="12">
         <f t="shared" si="9"/>
-        <v>-69</v>
+        <v>-70</v>
       </c>
       <c r="N10" s="13">
         <f t="shared" si="9"/>
-        <v>-136</v>
+        <v>-138</v>
       </c>
       <c r="O10" s="14">
         <f t="shared" si="9"/>
-        <v>-451</v>
+        <v>-458</v>
       </c>
       <c r="P10" s="15" t="s">
         <v>13</v>
@@ -2641,19 +2647,19 @@
       </c>
       <c r="L11" s="11">
         <f t="shared" ref="L11:O11" si="10">(G11-G17)+1</f>
-        <v>-14</v>
+        <v>-15</v>
       </c>
       <c r="M11" s="12">
         <f t="shared" si="10"/>
-        <v>-62</v>
+        <v>-63</v>
       </c>
       <c r="N11" s="13">
         <f t="shared" si="10"/>
-        <v>-122</v>
+        <v>-124</v>
       </c>
       <c r="O11" s="14">
         <f t="shared" si="10"/>
-        <v>-412</v>
+        <v>-419</v>
       </c>
       <c r="P11" s="15" t="s">
         <v>14</v>
@@ -2705,19 +2711,19 @@
       </c>
       <c r="L12" s="11">
         <f t="shared" ref="L12:O12" si="11">(G12-G17)+1</f>
-        <v>-22</v>
+        <v>-23</v>
       </c>
       <c r="M12" s="12">
         <f t="shared" si="11"/>
-        <v>-81</v>
+        <v>-82</v>
       </c>
       <c r="N12" s="13">
         <f t="shared" si="11"/>
-        <v>-162</v>
+        <v>-164</v>
       </c>
       <c r="O12" s="14">
         <f t="shared" si="11"/>
-        <v>-333</v>
+        <v>-340</v>
       </c>
       <c r="P12" s="15" t="s">
         <v>15</v>
@@ -2769,19 +2775,19 @@
       </c>
       <c r="L13" s="17">
         <f t="shared" ref="L13:O13" si="12">(G13-G17)+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M13" s="18">
         <f t="shared" si="12"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N13" s="19">
         <f t="shared" si="12"/>
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="O13" s="20">
         <f t="shared" si="12"/>
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="P13" s="15"/>
       <c r="Q13" s="6"/>
@@ -2831,19 +2837,19 @@
       </c>
       <c r="L14" s="17">
         <f t="shared" ref="L14:O14" si="13">(G14-G17)+1</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M14" s="18">
         <f t="shared" si="13"/>
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N14" s="19">
         <f t="shared" si="13"/>
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="O14" s="20">
         <f t="shared" si="13"/>
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="P14" s="15"/>
       <c r="Q14" s="6"/>
@@ -2897,19 +2903,19 @@
       </c>
       <c r="L15" s="17">
         <f t="shared" ref="L15:O15" si="15">(G15-G17)+1</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M15" s="18">
         <f t="shared" si="15"/>
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N15" s="19">
         <f t="shared" si="15"/>
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="O15" s="20">
         <f t="shared" si="15"/>
-        <v>925</v>
+        <v>918</v>
       </c>
       <c r="P15" s="15"/>
       <c r="Q15" s="6"/>
@@ -2963,19 +2969,19 @@
       </c>
       <c r="L16" s="17">
         <f t="shared" ref="L16:O16" si="17">(G16-G17)+1</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M16" s="18">
         <f t="shared" si="17"/>
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N16" s="19">
         <f t="shared" si="17"/>
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="O16" s="20">
         <f t="shared" si="17"/>
-        <v>629</v>
+        <v>622</v>
       </c>
       <c r="P16" s="15"/>
       <c r="Q16" s="6"/>
@@ -2994,35 +3000,35 @@
         <v>2024.0</v>
       </c>
       <c r="B17" s="25">
-        <v>169.0</v>
+        <v>170.0</v>
       </c>
       <c r="C17" s="25">
-        <v>1121.0</v>
+        <v>1122.0</v>
       </c>
       <c r="D17" s="25">
-        <v>2740.0</v>
+        <v>2742.0</v>
       </c>
       <c r="E17" s="25">
-        <v>9440.0</v>
+        <v>9447.0</v>
       </c>
       <c r="F17" s="25">
         <v>2024.0</v>
       </c>
       <c r="G17" s="26">
         <f t="shared" ref="G17:J17" si="18">B17-B16</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H17" s="26">
         <f t="shared" si="18"/>
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I17" s="26">
         <f t="shared" si="18"/>
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="J17" s="26">
         <f t="shared" si="18"/>
-        <v>891</v>
+        <v>898</v>
       </c>
       <c r="K17" s="10" t="s">
         <v>21</v>
@@ -33486,11 +33492,21 @@
       </c>
     </row>
     <row r="171">
-      <c r="A171" s="35"/>
-      <c r="B171" s="35"/>
-      <c r="C171" s="30"/>
-      <c r="D171" s="37"/>
-      <c r="E171" s="36"/>
+      <c r="A171" s="35">
+        <v>170.0</v>
+      </c>
+      <c r="B171" s="35" t="s">
+        <v>286</v>
+      </c>
+      <c r="C171" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="D171" s="35" t="s">
+        <v>287</v>
+      </c>
+      <c r="E171" s="36">
+        <v>0.008</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" s="35"/>

</xml_diff>